<commit_message>
update core , document
</commit_message>
<xml_diff>
--- a/Webadmin.xlsx
+++ b/Webadmin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452"/>
   </bookViews>
   <sheets>
     <sheet name="Màn hình chung" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Quản lý môn học" sheetId="6" r:id="rId7"/>
     <sheet name="Báo cáo thống kê" sheetId="7" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Báo cáo thống kê'!$D$2:$D$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="116">
   <si>
     <t>STT</t>
   </si>
@@ -60,9 +63,6 @@
     <t>View Modal</t>
   </si>
   <si>
-    <t>Danh sách giáo viên mới đăng kí chưa được xác nhận</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tên </t>
   </si>
   <si>
@@ -138,18 +138,6 @@
     <t>Báo cáo thống kê</t>
   </si>
   <si>
-    <t>Danh sách các lớp đang hoạt động</t>
-  </si>
-  <si>
-    <t>Chi tiết thông tin lớp ( số lượng học sinh )</t>
-  </si>
-  <si>
-    <t>Màn hình riêng biệt dạng list</t>
-  </si>
-  <si>
-    <t>Chi tiết thông tin điểm danh theo từng ngày của lớp</t>
-  </si>
-  <si>
     <t>Biểu đồ báo cáo doanh thu</t>
   </si>
   <si>
@@ -373,6 +361,27 @@
   </si>
   <si>
     <t>Khi tích vào check all thỳ lấy hết userId gửi lên service để thêm học sinh vào lớp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service : </t>
+  </si>
+  <si>
+    <t>Danh sách giáo viên mới đăng kí chưa được xác nhận ( UserType = 'D' )</t>
+  </si>
+  <si>
+    <t>Kiểu báo cáo</t>
+  </si>
+  <si>
+    <t>DAY - NGÀY</t>
+  </si>
+  <si>
+    <t>MONTH - THÁNG</t>
+  </si>
+  <si>
+    <t>YEAR- NĂM</t>
+  </si>
+  <si>
+    <t>Kiểu báo cáo sẽ là Key trước giá trị sau nó có dạng combobox và giao diện vẽ như kia</t>
   </si>
 </sst>
 </file>
@@ -474,6 +483,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>33897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1280160"/>
+          <a:ext cx="6713220" cy="3142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E18"/>
+  <dimension ref="A4:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,16 +811,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -787,21 +839,21 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -809,29 +861,29 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -839,21 +891,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -861,21 +913,21 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -883,37 +935,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -931,10 +959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E10"/>
+  <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +1006,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -989,13 +1017,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1003,13 +1031,18 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
       </c>
       <c r="E10">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1042,21 +1075,21 @@
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1064,22 +1097,22 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="H9" s="7"/>
     </row>
@@ -1091,10 +1124,10 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1199,12 +1232,12 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1214,25 +1247,25 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1242,27 +1275,27 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1272,10 +1305,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1285,10 +1318,10 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1298,10 +1331,10 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1311,10 +1344,10 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1324,10 +1357,10 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1366,21 +1399,21 @@
   <sheetData>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1388,28 +1421,28 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="J9" s="7"/>
     </row>
@@ -1423,10 +1456,10 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1551,12 +1584,12 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1566,10 +1599,10 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1578,15 +1611,15 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1598,10 +1631,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1610,17 +1643,17 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1632,10 +1665,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1647,10 +1680,10 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1662,10 +1695,10 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1677,10 +1710,10 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1692,10 +1725,10 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1707,10 +1740,10 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1722,10 +1755,10 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -1771,30 +1804,30 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1802,123 +1835,123 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1933,7 +1966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -1948,33 +1981,33 @@
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1982,59 +2015,59 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2059,15 +2092,15 @@
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2075,42 +2108,42 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2120,12 +2153,60 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="D2:D5">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Kiểu báo cáo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>